<commit_message>
code cleanup, replace text file
</commit_message>
<xml_diff>
--- a/make-elans-from-wavs-and-spreadsheet/input/test.xlsx
+++ b/make-elans-from-wavs-and-spreadsheet/input/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbb/sandbox/elan-helpers/make-elans-from-wavs-and-csv/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbb/sandbox/elan-helpers/make-elans-from-wavs-and-spreadsheet/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0D8F485-030F-6547-A1C6-2EA430427660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A528C783-4DAC-F746-A483-38D42B8A849B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{9B9FB471-94A0-7F49-8013-C3C3B4DB1616}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>File name</t>
   </si>
@@ -41,130 +41,28 @@
     <t>Transcription</t>
   </si>
   <si>
-    <t>Translation (machine generated)</t>
-  </si>
-  <si>
-    <t>Date/time</t>
-  </si>
-  <si>
-    <t>Length (milliseconds)</t>
-  </si>
-  <si>
-    <t>Bitrate (bytes/second)</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Filetype</t>
-  </si>
-  <si>
-    <t>Speaker name</t>
-  </si>
-  <si>
-    <t>Native language</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Checked?</t>
-  </si>
-  <si>
-    <t>Validated?</t>
-  </si>
-  <si>
-    <t>vMUrWEM1FlegHdc.wav</t>
-  </si>
-  <si>
     <t>yuwa</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>2020-02-25 15:17:58</t>
-  </si>
-  <si>
-    <t>1707</t>
-  </si>
-  <si>
-    <t>11025</t>
-  </si>
-  <si>
-    <t>Realtek High Definition Audio</t>
-  </si>
-  <si>
-    <t>Alice Springs</t>
-  </si>
-  <si>
-    <t>Wave</t>
-  </si>
-  <si>
-    <t>Brendan Kavanagh</t>
-  </si>
-  <si>
-    <t>Brendan</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>OdbBRezmQi4KBLs.wav</t>
-  </si>
-  <si>
     <t>palya</t>
   </si>
   <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>2020-02-25 15:18:10</t>
-  </si>
-  <si>
-    <t>1017</t>
-  </si>
-  <si>
-    <t>5Nx1SNjV6zlE6U4.wav</t>
-  </si>
-  <si>
     <t>kuya</t>
   </si>
   <si>
-    <t>Bad</t>
-  </si>
-  <si>
-    <t>2020-02-25 15:18:24</t>
-  </si>
-  <si>
-    <t>2177</t>
-  </si>
-  <si>
-    <t>USMvxXI7895E2aw.wav</t>
-  </si>
-  <si>
     <t>wiya</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>2020-02-25 15:18:36</t>
-  </si>
-  <si>
-    <t>1197</t>
+    <t>1.wav</t>
+  </si>
+  <si>
+    <t>2.wav</t>
+  </si>
+  <si>
+    <t>3.wav</t>
+  </si>
+  <si>
+    <t>4.wav</t>
   </si>
 </sst>
 </file>
@@ -522,247 +420,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B132D22-FD46-F642-A36D-F6A37E9D7BB3}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>